<commit_message>
separating login test in a login file , creating a login and postRequest gui
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tarek Radwan\Documents\NetBeansProjects\RentUpTesting1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FB3498-2B49-408B-9B53-B01371CA114F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7265DA81-5EA6-4071-863F-88E9C124FDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="570" windowWidth="11520" windowHeight="10350" xr2:uid="{141874D1-7D9B-4141-8C8D-C24D2395C610}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{141874D1-7D9B-4141-8C8D-C24D2395C610}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,34 +33,188 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="58">
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>mohamedtarek20196046@gmail.com</t>
-  </si>
-  <si>
-    <t>Mido2001</t>
+    <t>test123@gmail.com</t>
+  </si>
+  <si>
+    <t>mido</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>City</t>
   </si>
   <si>
     <t>District</t>
   </si>
   <si>
+    <t>neighbourhood</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Duration number</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Budget</t>
+  </si>
+  <si>
+    <t>Furnishing status</t>
+  </si>
+  <si>
+    <t>Minimum rooms</t>
+  </si>
+  <si>
+    <t>Property types</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
     <t>Masr El Gedida</t>
   </si>
   <si>
-    <t>Budget</t>
+    <t>Almazah</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">will get pet </t>
+  </si>
+  <si>
+    <t>term 1</t>
+  </si>
+  <si>
+    <t>term 2</t>
+  </si>
+  <si>
+    <t>term 3</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NA</t>
+  </si>
+  <si>
+    <t>Unfurnished</t>
+  </si>
+  <si>
+    <t>studio</t>
+  </si>
+  <si>
+    <t>Name+J7A1:L7</t>
+  </si>
+  <si>
+    <t>Giza</t>
+  </si>
+  <si>
+    <t>Alexanderia</t>
+  </si>
+  <si>
+    <t>Luxor</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>West Somid</t>
+  </si>
+  <si>
+    <t>Dahab</t>
+  </si>
+  <si>
+    <t>Canyon</t>
+  </si>
+  <si>
+    <t>Tropitel</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>Zamalek</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>Blue Hole</t>
+  </si>
+  <si>
+    <t>Allow smoking</t>
+  </si>
+  <si>
+    <t>Free WiFi</t>
+  </si>
+  <si>
+    <t>Mobile charger</t>
+  </si>
+  <si>
+    <t>Serviced Apartment</t>
+  </si>
+  <si>
+    <t>Maadi</t>
+  </si>
+  <si>
+    <t>Cornich El Maadi</t>
+  </si>
+  <si>
+    <t>nights</t>
+  </si>
+  <si>
+    <t>Duplex</t>
+  </si>
+  <si>
+    <t>Villa</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>Furnished</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,6 +235,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,10 +267,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -426,61 +596,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1098C183-8FAE-4F9D-B3E2-C948E79AEC1D}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>333</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>333</v>
-      </c>
+      <c r="L5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1651651</v>
-      </c>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{1C5D1A22-CAFC-4658-A3BA-D51C443180CA}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{1A1EA47F-A813-44C6-9E00-EBB1A4C47C2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add listing panel 2
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tarek Radwan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Omar Fekry\Documents\NetBeansProjects\RentUpTesting\RentUpTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{176A2214-A2E6-4949-92A0-5213181A1772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40A4711-E4C2-4CA0-9440-583709585D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{141874D1-7D9B-4141-8C8D-C24D2395C610}"/>
+    <workbookView xWindow="14055" yWindow="2715" windowWidth="14205" windowHeight="11295" xr2:uid="{141874D1-7D9B-4141-8C8D-C24D2395C610}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -41,21 +41,78 @@
     <t>Password</t>
   </si>
   <si>
-    <t>mohamedtarek20196046@gmail.com</t>
-  </si>
-  <si>
-    <t>Mido2001</t>
+    <t>District</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Search Key</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>arvknkh5m@mozmail.com</t>
+  </si>
+  <si>
+    <t>Add Listing</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Furnishing status</t>
+  </si>
+  <si>
+    <t>Property type</t>
+  </si>
+  <si>
+    <t>Number of rooms</t>
+  </si>
+  <si>
+    <t>Number of bathrooms</t>
+  </si>
+  <si>
+    <t>Property name</t>
+  </si>
+  <si>
+    <t>Rent / night</t>
+  </si>
+  <si>
+    <t>Rent / month</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>autolandlord@1.com</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -64,9 +121,16 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -91,9 +155,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,46 +477,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1098C183-8FAE-4F9D-B3E2-C948E79AEC1D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="P3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="P8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="P9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="P13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1651651</v>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>123456</v>
+      </c>
+      <c r="P15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F21" t="str">
+        <f>0</f>
+        <v>tttt</v>
+      </c>
+      <c r="P21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{1C5D1A22-CAFC-4658-A3BA-D51C443180CA}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{1A1EA47F-A813-44C6-9E00-EBB1A4C47C2D}"/>
-  </hyperlinks>
+  <mergeCells count="2">
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mig Landlord - Delete Tenant in Adminpanel are done (v2)
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farida Osama\Desktop\Rentup\"/>
     </mc:Choice>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="83">
   <si>
     <t>Name+J7A1:L7</t>
   </si>
@@ -229,12 +229,58 @@
   </si>
   <si>
     <t>some integer condition altered to radio</t>
+  </si>
+  <si>
+    <t>rWVCYp4YUX@test.com</t>
+  </si>
+  <si>
+    <t>tR1HRg9erV@test.com</t>
+  </si>
+  <si>
+    <t>magdaosama@test.com</t>
+  </si>
+  <si>
+    <t>UhCTimSJYX@test.com</t>
+  </si>
+  <si>
+    <t>BQ9TPxeA81@test.com</t>
+  </si>
+  <si>
+    <t>oWZ4gNhJZ5@test.com</t>
+  </si>
+  <si>
+    <t>YEQBHzMhmj@test.com</t>
+  </si>
+  <si>
+    <t>7MTVYJOtxr@test.com</t>
+  </si>
+  <si>
+    <t>LZD8sRo9ov@test.com</t>
+  </si>
+  <si>
+    <t>mPjnO2GV6T@test.com</t>
+  </si>
+  <si>
+    <t>kinOZXRMCV@test.com</t>
+  </si>
+  <si>
+    <t>TXA9sTo7hG@test.com</t>
+  </si>
+  <si>
+    <t>SZphrxC2Zl@test.com</t>
+  </si>
+  <si>
+    <t>bHJi2rfBCj@test.com</t>
+  </si>
+  <si>
+    <t>Z0h3EH6beg@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="12"/>
@@ -567,21 +613,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.6328125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.453125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.6328125" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="8.453125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.90625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.54296875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.36328125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.90625" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="20.36328125" customWidth="1" collapsed="1"/>
-    <col min="17" max="27" width="8.453125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.81640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.1796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.90625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.6328125" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="8.453125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.36328125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="14.90625" collapsed="true"/>
+    <col min="15" max="16" customWidth="true" width="20.36328125" collapsed="true"/>
+    <col min="17" max="27" customWidth="true" width="8.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -943,7 +989,7 @@
         <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
         <v>57</v>
@@ -1008,7 +1054,7 @@
         <v>52</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2">
         <v>123456</v>

</xml_diff>